<commit_message>
added more selenium stuff
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -1,22 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\automated_testing\udemy_course\java-selenium-training\src\test\resources\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mikalai_biadrytski/Documents/autotests/udemy/java-selenium-training/src/test/resources/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
+    <workbookView xWindow="40620" yWindow="1480" windowWidth="26840" windowHeight="15120" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="AddCustomerTest" sheetId="1" r:id="rId1"/>
+    <sheet name="test_suite" sheetId="3" r:id="rId2"/>
+    <sheet name="OpenAccountTest" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
   <si>
     <t>firstname</t>
   </si>
@@ -45,19 +53,73 @@
   </si>
   <si>
     <t>Customer added successfully</t>
+  </si>
+  <si>
+    <t>customer</t>
+  </si>
+  <si>
+    <t>currency</t>
+  </si>
+  <si>
+    <t>Nick Hero</t>
+  </si>
+  <si>
+    <t>Rupee</t>
+  </si>
+  <si>
+    <t>Nick1</t>
+  </si>
+  <si>
+    <t>Nick2</t>
+  </si>
+  <si>
+    <t>Nick3</t>
+  </si>
+  <si>
+    <t>Hero1</t>
+  </si>
+  <si>
+    <t>Hero2</t>
+  </si>
+  <si>
+    <t>Hero3</t>
+  </si>
+  <si>
+    <t>TCID</t>
+  </si>
+  <si>
+    <t>Runmode</t>
+  </si>
+  <si>
+    <t>BankManagerLoginTest</t>
+  </si>
+  <si>
+    <t>AddCustomerTest</t>
+  </si>
+  <si>
+    <t>OpenAccountTest</t>
+  </si>
+  <si>
+    <t>Y</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Menlo"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -80,11 +142,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -362,46 +425,169 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.83203125" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" customWidth="1"/>
+    <col min="3" max="3" width="15.5" customWidth="1"/>
+    <col min="4" max="4" width="26.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>223098</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3">
+        <v>223098</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4">
+        <v>223098</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5">
+        <v>223098</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" customWidth="1"/>
-    <col min="4" max="4" width="26.85546875" customWidth="1"/>
+    <col min="1" max="1" width="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2">
-        <v>223098</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>